<commit_message>
Got lab06 as far as I could before running into a critical error that was never able to be solved in any lab.
</commit_message>
<xml_diff>
--- a/homework/Reviews/memberReview.xlsx
+++ b/homework/Reviews/memberReview.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Review 1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Review 2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Review 3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="21">
   <si>
     <t xml:space="preserve">Homework 1</t>
   </si>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 3</t>
   </si>
 </sst>
 </file>
@@ -155,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +186,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -858,8 +866,8 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1480,6 +1488,696 @@
       </c>
       <c r="D61" s="1" t="n">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A43:A51"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A53:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="6" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>